<commit_message>
Actualicé app.py, nuevas plantillas y archivos de ejemplo
</commit_message>
<xml_diff>
--- a/uploads/resultados.xlsx
+++ b/uploads/resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>Predicción</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Probabilidad</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -482,6 +487,9 @@
         <v>15</v>
       </c>
       <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -504,6 +512,9 @@
       <c r="F3" t="n">
         <v>0</v>
       </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -524,6 +535,9 @@
       <c r="F4" t="n">
         <v>0</v>
       </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -542,6 +556,9 @@
         <v>10</v>
       </c>
       <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -564,6 +581,9 @@
       <c r="F6" t="n">
         <v>1</v>
       </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -584,6 +604,9 @@
       <c r="F7" t="n">
         <v>0</v>
       </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -604,6 +627,9 @@
       <c r="F8" t="n">
         <v>1</v>
       </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -622,6 +648,9 @@
         <v>14</v>
       </c>
       <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -644,6 +673,9 @@
       <c r="F10" t="n">
         <v>0</v>
       </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -662,6 +694,9 @@
         <v>11</v>
       </c>
       <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>